<commit_message>
Optimal LLM query, One sheet for Q & results
</commit_message>
<xml_diff>
--- a/data/IPIPDatasetWithScores.xlsx
+++ b/data/IPIPDatasetWithScores.xlsx
@@ -34713,4 +34713,10 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>